<commit_message>
finalizado hasta results std
Todo std, solo falta exportar a excel
</commit_message>
<xml_diff>
--- a/Resultados_auto.xlsx
+++ b/Resultados_auto.xlsx
@@ -13,7 +13,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+  <si>
+    <t>Linear Nic</t>
+  </si>
+  <si>
+    <t>Linear USA</t>
+  </si>
+  <si>
+    <t>Quadratic Nic</t>
+  </si>
+  <si>
+    <t>Quadratic USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 USA</t>
+  </si>
+  <si>
+    <t>Linear Nic</t>
+  </si>
+  <si>
+    <t>Linear USA</t>
+  </si>
+  <si>
+    <t>Quadratic Nic</t>
+  </si>
+  <si>
+    <t>Quadratic USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 USA</t>
+  </si>
+  <si>
+    <t>Linear Nic</t>
+  </si>
+  <si>
+    <t>Linear USA</t>
+  </si>
+  <si>
+    <t>Quadratic Nic</t>
+  </si>
+  <si>
+    <t>Quadratic USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 USA</t>
+  </si>
   <si>
     <t>Linear Nic</t>
   </si>
@@ -85,40 +157,40 @@
   <dimension ref="A1:H7"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="true"/>
+    <col min="1" max="1" width="13.37890625" customWidth="true"/>
     <col min="2" max="2" width="12.7109375" customWidth="true"/>
-    <col min="3" max="3" width="13.42578125" customWidth="true"/>
-    <col min="4" max="4" width="14.42578125" customWidth="true"/>
-    <col min="5" max="5" width="16.7109375" customWidth="true"/>
-    <col min="6" max="6" width="17.42578125" customWidth="true"/>
-    <col min="7" max="7" width="17.28515625" customWidth="true"/>
-    <col min="8" max="8" width="18" customWidth="true"/>
+    <col min="3" max="3" width="13.37890625" customWidth="true"/>
+    <col min="4" max="4" width="14.37890625" customWidth="true"/>
+    <col min="5" max="5" width="16.15625" customWidth="true"/>
+    <col min="6" max="6" width="16.82421875" customWidth="true"/>
+    <col min="7" max="7" width="16.7109375" customWidth="true"/>
+    <col min="8" max="8" width="17.37890625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
results std to excel
Hasta exportacion en excel de standard deviation
</commit_message>
<xml_diff>
--- a/Resultados_auto.xlsx
+++ b/Resultados_auto.xlsx
@@ -13,7 +13,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+  <si>
+    <t>Linear Nic</t>
+  </si>
+  <si>
+    <t>Linear USA</t>
+  </si>
+  <si>
+    <t>Quadratic Nic</t>
+  </si>
+  <si>
+    <t>Quadratic USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 USA</t>
+  </si>
+  <si>
+    <t>Linear Nic</t>
+  </si>
+  <si>
+    <t>Linear USA</t>
+  </si>
+  <si>
+    <t>Quadratic Nic</t>
+  </si>
+  <si>
+    <t>Quadratic USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 USA</t>
+  </si>
+  <si>
+    <t>Linear Nic</t>
+  </si>
+  <si>
+    <t>Linear USA</t>
+  </si>
+  <si>
+    <t>Quadratic Nic</t>
+  </si>
+  <si>
+    <t>Quadratic USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 USA</t>
+  </si>
   <si>
     <t>Linear Nic</t>
   </si>
@@ -169,28 +241,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
rounding to nearest hundredth
-Rounding
</commit_message>
<xml_diff>
--- a/Resultados_auto.xlsx
+++ b/Resultados_auto.xlsx
@@ -13,7 +13,103 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+  <si>
+    <t>Linear Nic</t>
+  </si>
+  <si>
+    <t>Linear USA</t>
+  </si>
+  <si>
+    <t>Quadratic Nic</t>
+  </si>
+  <si>
+    <t>Quadratic USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 USA</t>
+  </si>
+  <si>
+    <t>Linear Nic</t>
+  </si>
+  <si>
+    <t>Linear USA</t>
+  </si>
+  <si>
+    <t>Quadratic Nic</t>
+  </si>
+  <si>
+    <t>Quadratic USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 USA</t>
+  </si>
+  <si>
+    <t>Linear Nic</t>
+  </si>
+  <si>
+    <t>Linear USA</t>
+  </si>
+  <si>
+    <t>Quadratic Nic</t>
+  </si>
+  <si>
+    <t>Quadratic USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 USA</t>
+  </si>
+  <si>
+    <t>Linear Nic</t>
+  </si>
+  <si>
+    <t>Linear USA</t>
+  </si>
+  <si>
+    <t>Quadratic Nic</t>
+  </si>
+  <si>
+    <t>Quadratic USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 USA</t>
+  </si>
   <si>
     <t>Linear Nic</t>
   </si>
@@ -241,28 +337,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
22 de junio a las 10:17
- agrego ciclos a usa
- calculo duracion y magnitu promedio y tabla excel
- codigos de dinare
</commit_message>
<xml_diff>
--- a/Resultados_auto.xlsx
+++ b/Resultados_auto.xlsx
@@ -13,7 +13,127 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="400">
+  <si>
+    <t>Linear Nic</t>
+  </si>
+  <si>
+    <t>Linear USA</t>
+  </si>
+  <si>
+    <t>Quadratic Nic</t>
+  </si>
+  <si>
+    <t>Quadratic USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 USA</t>
+  </si>
+  <si>
+    <t>Linear Nic</t>
+  </si>
+  <si>
+    <t>Linear USA</t>
+  </si>
+  <si>
+    <t>Quadratic Nic</t>
+  </si>
+  <si>
+    <t>Quadratic USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 USA</t>
+  </si>
+  <si>
+    <t>Linear Nic</t>
+  </si>
+  <si>
+    <t>Linear USA</t>
+  </si>
+  <si>
+    <t>Quadratic Nic</t>
+  </si>
+  <si>
+    <t>Quadratic USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 USA</t>
+  </si>
+  <si>
+    <t>Linear Nic</t>
+  </si>
+  <si>
+    <t>Linear USA</t>
+  </si>
+  <si>
+    <t>Quadratic Nic</t>
+  </si>
+  <si>
+    <t>Quadratic USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 USA</t>
+  </si>
+  <si>
+    <t>Linear Nic</t>
+  </si>
+  <si>
+    <t>Linear USA</t>
+  </si>
+  <si>
+    <t>Quadratic Nic</t>
+  </si>
+  <si>
+    <t>Quadratic USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 100 USA</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 Nic</t>
+  </si>
+  <si>
+    <t>HP con λ = 6.25 USA</t>
+  </si>
   <si>
     <t>Linear Nic</t>
   </si>
@@ -1153,28 +1273,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>352</v>
+        <v>392</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>353</v>
+        <v>393</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>354</v>
+        <v>394</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>355</v>
+        <v>395</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>356</v>
+        <v>396</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>357</v>
+        <v>397</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>358</v>
+        <v>398</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>359</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2">

</xml_diff>